<commit_message>
Visible Raid Points update
가독성
</commit_message>
<xml_diff>
--- a/Pull Request Here/Visible Raid Points - 2562730174/Visible Raid Points - 2562730174.xlsx
+++ b/Pull Request Here/Visible Raid Points - 2562730174/Visible Raid Points - 2562730174.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\Visible Raid Points - 2562730174\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEC3C3D-C33D-44AB-AFA6-BC659FC4CD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FA15E3-B0A3-49E0-A212-354A23521567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1126,22 +1126,10 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>재산에 따라 증가함</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>위협 점수</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>계산되는 정착민들</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>포인트 (계산된 정착민들의 합계)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>시작값</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1371,6 +1359,18 @@
   </si>
   <si>
     <t>해당 세력의 전략: {0} 포인트로 계산합니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>재산에 따라 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>계산되는 정착민과 동물들</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>포인트 (계산된 정착민과 동물들의 합계)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1813,7 +1813,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1830,7 +1830,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1847,7 +1847,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1864,7 +1864,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2020,7 +2020,7 @@
         <v>299</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2156,7 +2156,7 @@
         <v>247</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>295</v>
@@ -2570,7 +2570,7 @@
         <v>322</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2587,7 +2587,7 @@
         <v>293</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>295</v>
@@ -2607,7 +2607,7 @@
         <v>323</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2621,10 +2621,10 @@
         <v>104</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2641,7 +2641,7 @@
         <v>107</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2658,7 +2658,7 @@
         <v>110</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>333</v>
+        <v>391</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2675,7 +2675,7 @@
         <v>325</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>331</v>
+        <v>390</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2692,7 +2692,7 @@
         <v>115</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>334</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2709,7 +2709,7 @@
         <v>118</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>295</v>
@@ -2729,7 +2729,7 @@
         <v>121</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -2746,7 +2746,7 @@
         <v>124</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -2763,7 +2763,7 @@
         <v>326</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2797,7 +2797,7 @@
         <v>222</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -2814,7 +2814,7 @@
         <v>132</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -2828,10 +2828,10 @@
         <v>134</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>295</v>
@@ -2888,7 +2888,7 @@
         <v>220</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2905,7 +2905,7 @@
         <v>143</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2922,7 +2922,7 @@
         <v>221</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2939,7 +2939,7 @@
         <v>304</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2973,7 +2973,7 @@
         <v>150</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>295</v>
@@ -2993,7 +2993,7 @@
         <v>153</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -3010,7 +3010,7 @@
         <v>156</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>295</v>
@@ -3030,7 +3030,7 @@
         <v>159</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3081,7 +3081,7 @@
         <v>314</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3098,7 +3098,7 @@
         <v>315</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3115,7 +3115,7 @@
         <v>316</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3132,7 +3132,7 @@
         <v>317</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3149,7 +3149,7 @@
         <v>174</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3166,7 +3166,7 @@
         <v>318</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3180,10 +3180,10 @@
         <v>178</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3200,7 +3200,7 @@
         <v>302</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>295</v>
@@ -3220,7 +3220,7 @@
         <v>183</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>295</v>
@@ -3237,7 +3237,7 @@
         <v>185</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>251</v>
@@ -3254,10 +3254,10 @@
         <v>187</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3274,7 +3274,7 @@
         <v>190</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3291,7 +3291,7 @@
         <v>193</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3308,7 +3308,7 @@
         <v>196</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3322,10 +3322,10 @@
         <v>198</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3342,7 +3342,7 @@
         <v>201</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3359,7 +3359,7 @@
         <v>204</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3376,7 +3376,7 @@
         <v>207</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3393,7 +3393,7 @@
         <v>210</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3404,13 +3404,13 @@
         <v>7</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>295</v>
@@ -3427,10 +3427,10 @@
         <v>213</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -3444,10 +3444,10 @@
         <v>215</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -3461,10 +3461,10 @@
         <v>217</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -3478,13 +3478,13 @@
         <v>219</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>299</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>